<commit_message>
Update README to explain zipped files may affect file paths & advised NOT to run the initial individual student EDA files as they are early, exploratory files that do not have supporting datasets uploaded.
Updated project tracker to reflect time spent on Git issues
</commit_message>
<xml_diff>
--- a/code_first_girls_project_documents /Group Seven Project Activity Log.xlsx
+++ b/code_first_girls_project_documents /Group Seven Project Activity Log.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="183">
   <si>
     <r>
       <rPr>
@@ -1020,6 +1020,23 @@
     <t>Final edit of project document to meet length requirements</t>
   </si>
   <si>
+    <t>Lottie - GitHub Project Submission Issues</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Git trouble - Git pull/push error: RPC failed; result=22, HTTP code = 408 - fix = git config http.postBuffer 500000000, git config http.lowSpeedTime 600 - then: files to large, suggested using Git LFS (large file storage), selected .csv &amp; .csv.gz files to convert to LFS, commit = fail &gt; repo over storage limit! - Delete large files we didn't need in the repo = git push --force ... nothing.... | create new branch 'project_submission' to divert from previous commits, push new branch... 
+remote: error: File data/csv/airbnb_datasets/airbnb_files_raw_uncleansed/detailed_listings_scraped_March23.csv is 170.39 MB; this exceeds GitHub's file size limit of 100.00 MB        
+remote: error: File archived_files/other/airbnb_combined_data_quality_check.csv is 319.28 MB; this exceeds GitHub's file size limit of 100.00 MB        
+remote: error: File data/csv/airbnb_datasets/files_not_used/reviews.csv.gz is 151.52 MB; this exceeds GitHub's file size limit of 100.00 MB        
+remote: error: File data/csv/airbnb_datasets/airbnb_files_raw_uncleansed/detailed_listings_scraped_June22.csv is 146.45 MB; this exceeds GitHub's file size limit of 100.00 MB        
+remote: error: GH001: Large files detected. You may want to try Git Large File Storage - https://git-lfs.github.com.        
+error: failed to push some refs to 'https://github.com/LottieJane1312/cfg_data2_group7_project.git'
+Not sure what to do now....  rebased to 'main' - undo commits : zipped/deleted large files - pushed repo without them - WORKED! - git.add zipped files - pushed... WORKED! 
+NB: Not sure how zipping the files will effect the running of the Notebooks but there's literally nothing I can do about it so please Kosi can you unzip when you clone the repo if this causes an issue. Thanks! - EDITED README. to give this info</t>
+  </si>
+  <si>
     <t>Lottie - Final Submission</t>
   </si>
   <si>
@@ -5524,19 +5541,19 @@
         <v>5.0</v>
       </c>
       <c r="B102" s="21">
-        <v>410315.0</v>
+        <v>45073.0</v>
       </c>
       <c r="C102" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D102" s="23">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="E102" s="23" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="F102" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -5560,65 +5577,77 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103">
-      <c r="A103" s="39"/>
-      <c r="B103" s="40"/>
-      <c r="C103" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D103" s="39">
-        <f>SUM(D8:D102)</f>
-        <v>11920</v>
-      </c>
-      <c r="E103" s="39"/>
-      <c r="F103" s="42"/>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
-      <c r="J103" s="18"/>
-      <c r="K103" s="18"/>
-      <c r="L103" s="18"/>
-      <c r="M103" s="43"/>
-      <c r="N103" s="43"/>
-      <c r="O103" s="43"/>
-      <c r="P103" s="43"/>
-      <c r="Q103" s="43"/>
-      <c r="R103" s="43"/>
-      <c r="S103" s="43"/>
-      <c r="T103" s="43"/>
-      <c r="U103" s="43"/>
-      <c r="V103" s="43"/>
-      <c r="W103" s="43"/>
-      <c r="X103" s="43"/>
-      <c r="Y103" s="43"/>
-      <c r="Z103" s="43"/>
+      <c r="A103" s="23">
+        <v>5.0</v>
+      </c>
+      <c r="B103" s="21">
+        <v>410315.0</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D103" s="23">
+        <v>240.0</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="2"/>
+      <c r="T103" s="2"/>
+      <c r="U103" s="2"/>
+      <c r="V103" s="2"/>
+      <c r="W103" s="2"/>
+      <c r="X103" s="2"/>
+      <c r="Y103" s="2"/>
+      <c r="Z103" s="2"/>
     </row>
     <row r="104">
-      <c r="A104" s="44"/>
-      <c r="B104" s="45"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="44"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
-      <c r="N104" s="2"/>
-      <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
-      <c r="Q104" s="2"/>
-      <c r="R104" s="2"/>
-      <c r="S104" s="2"/>
-      <c r="T104" s="2"/>
-      <c r="U104" s="2"/>
-      <c r="V104" s="2"/>
-      <c r="W104" s="2"/>
-      <c r="X104" s="2"/>
-      <c r="Y104" s="2"/>
-      <c r="Z104" s="2"/>
+      <c r="A104" s="39"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D104" s="39">
+        <f>SUM(D8:D103)</f>
+        <v>12130</v>
+      </c>
+      <c r="E104" s="39"/>
+      <c r="F104" s="42"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="18"/>
+      <c r="M104" s="43"/>
+      <c r="N104" s="43"/>
+      <c r="O104" s="43"/>
+      <c r="P104" s="43"/>
+      <c r="Q104" s="43"/>
+      <c r="R104" s="43"/>
+      <c r="S104" s="43"/>
+      <c r="T104" s="43"/>
+      <c r="U104" s="43"/>
+      <c r="V104" s="43"/>
+      <c r="W104" s="43"/>
+      <c r="X104" s="43"/>
+      <c r="Y104" s="43"/>
+      <c r="Z104" s="43"/>
     </row>
     <row r="105">
       <c r="A105" s="44"/>
@@ -5901,12 +5930,12 @@
       <c r="Z114" s="2"/>
     </row>
     <row r="115">
-      <c r="A115" s="46"/>
-      <c r="B115" s="47"/>
-      <c r="C115" s="46"/>
-      <c r="D115" s="48"/>
-      <c r="E115" s="48"/>
-      <c r="F115" s="10"/>
+      <c r="A115" s="44"/>
+      <c r="B115" s="45"/>
+      <c r="C115" s="44"/>
+      <c r="D115" s="44"/>
+      <c r="E115" s="44"/>
+      <c r="F115" s="6"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -6069,12 +6098,12 @@
       <c r="Z120" s="2"/>
     </row>
     <row r="121">
-      <c r="A121" s="5"/>
-      <c r="B121" s="49"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="51"/>
-      <c r="E121" s="51"/>
-      <c r="F121" s="52"/>
+      <c r="A121" s="46"/>
+      <c r="B121" s="47"/>
+      <c r="C121" s="46"/>
+      <c r="D121" s="48"/>
+      <c r="E121" s="48"/>
+      <c r="F121" s="10"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -6330,7 +6359,7 @@
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
-      <c r="J130" s="53"/>
+      <c r="J130" s="2"/>
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
       <c r="M130" s="2"/>
@@ -6358,7 +6387,7 @@
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
-      <c r="J131" s="54"/>
+      <c r="J131" s="53"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
@@ -6386,7 +6415,7 @@
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
-      <c r="J132" s="53"/>
+      <c r="J132" s="54"/>
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
       <c r="M132" s="2"/>
@@ -7030,7 +7059,7 @@
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
-      <c r="J155" s="2"/>
+      <c r="J155" s="53"/>
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
       <c r="M155" s="2"/>
@@ -7552,12 +7581,12 @@
       <c r="Y173" s="2"/>
       <c r="Z173" s="2"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="2"/>
-      <c r="B174" s="55"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="15"/>
-      <c r="E174" s="15"/>
+    <row r="174">
+      <c r="A174" s="5"/>
+      <c r="B174" s="49"/>
+      <c r="C174" s="50"/>
+      <c r="D174" s="51"/>
+      <c r="E174" s="51"/>
       <c r="F174" s="52"/>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -32695,6 +32724,34 @@
       <c r="X1071" s="2"/>
       <c r="Y1071" s="2"/>
       <c r="Z1071" s="2"/>
+    </row>
+    <row r="1072" ht="15.75" customHeight="1">
+      <c r="A1072" s="2"/>
+      <c r="B1072" s="55"/>
+      <c r="C1072" s="2"/>
+      <c r="D1072" s="15"/>
+      <c r="E1072" s="15"/>
+      <c r="F1072" s="52"/>
+      <c r="G1072" s="2"/>
+      <c r="H1072" s="2"/>
+      <c r="I1072" s="2"/>
+      <c r="J1072" s="2"/>
+      <c r="K1072" s="2"/>
+      <c r="L1072" s="2"/>
+      <c r="M1072" s="2"/>
+      <c r="N1072" s="2"/>
+      <c r="O1072" s="2"/>
+      <c r="P1072" s="2"/>
+      <c r="Q1072" s="2"/>
+      <c r="R1072" s="2"/>
+      <c r="S1072" s="2"/>
+      <c r="T1072" s="2"/>
+      <c r="U1072" s="2"/>
+      <c r="V1072" s="2"/>
+      <c r="W1072" s="2"/>
+      <c r="X1072" s="2"/>
+      <c r="Y1072" s="2"/>
+      <c r="Z1072" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>